<commit_message>
fix(portfolio): correct TWR calculation by simplifying shares computation
Refactor shares calculation to use net cash flow divided by NAV, which fixes incorrect TWR results. Update test data to reflect accurate calculations.
</commit_message>
<xml_diff>
--- a/tests/output/twr_daily_correct.xlsx
+++ b/tests/output/twr_daily_correct.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -64,10 +64,13 @@
     <t>nav_today</t>
   </si>
   <si>
-    <t>nav_prev</t>
+    <t>shares_today</t>
   </si>
   <si>
-    <t>shares_today</t>
+    <t>delta_cf</t>
+  </si>
+  <si>
+    <t>nav_prev</t>
   </si>
   <si>
     <t>shares_prev</t>
@@ -242,12 +245,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -568,7 +577,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -592,16 +601,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -610,96 +619,105 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1013,10 +1031,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q47"/>
+  <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1027,9 +1045,14 @@
     <col min="7" max="7" width="13.75" customWidth="1"/>
     <col min="8" max="8" width="9.375" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="9" style="1"/>
+    <col min="11" max="11" width="10.375" style="2" customWidth="1"/>
+    <col min="12" max="14" width="13.75" customWidth="1"/>
+    <col min="15" max="15" width="12.125" customWidth="1"/>
+    <col min="18" max="18" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1057,33 +1080,42 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="1">
+      <c r="T1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="3">
         <v>45658</v>
       </c>
       <c r="B2">
@@ -1110,34 +1142,43 @@
       <c r="I2">
         <v>3.9</v>
       </c>
-      <c r="J2">
-        <f t="shared" ref="J2:J47" si="0">B2+C2+D2*G2+E2*H2*0.92+F2*I2</f>
+      <c r="J2" s="1">
+        <f t="shared" ref="J2:J47" si="0">B2+C2*0.92+D2*G2+E2*H2*0.92+F2*I2</f>
         <v>300000</v>
       </c>
       <c r="K2" s="2">
         <v>1</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2">
+        <v>300000</v>
+      </c>
+      <c r="M2">
+        <v>300000</v>
+      </c>
+      <c r="N2" s="4">
         <v>1</v>
       </c>
-      <c r="M2" s="2">
-        <v>300000</v>
-      </c>
-      <c r="N2" s="2">
-        <v>300000</v>
-      </c>
-      <c r="O2" s="2">
-        <v>300000</v>
-      </c>
-      <c r="P2" s="2">
-        <v>300000</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="1">
+      <c r="O2" s="4">
+        <v>1</v>
+      </c>
+      <c r="P2" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R2" s="5">
+        <v>300000</v>
+      </c>
+      <c r="S2" s="4">
+        <v>300000</v>
+      </c>
+      <c r="T2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="3">
         <v>45659</v>
       </c>
       <c r="B3">
@@ -1164,34 +1205,45 @@
       <c r="I3">
         <v>3.9</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <f t="shared" si="0"/>
         <v>300000</v>
       </c>
       <c r="K3" s="2">
+        <f>(J3-M3)/L2</f>
         <v>1</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3">
+        <f>L2+M3/K3</f>
+        <v>300000</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4">
         <v>1</v>
       </c>
-      <c r="M3" s="2">
-        <v>300000</v>
-      </c>
-      <c r="N3" s="2">
-        <v>300000</v>
-      </c>
-      <c r="O3" s="2">
-        <v>300000</v>
-      </c>
-      <c r="P3" s="2">
-        <v>300000</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="1">
+      <c r="O3" s="4">
+        <v>1</v>
+      </c>
+      <c r="P3" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R3" s="5">
+        <v>300000</v>
+      </c>
+      <c r="S3" s="4">
+        <v>300000</v>
+      </c>
+      <c r="T3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="3">
         <v>45660</v>
       </c>
       <c r="B4">
@@ -1218,34 +1270,45 @@
       <c r="I4">
         <v>3.9</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="1">
         <f t="shared" si="0"/>
         <v>300000</v>
       </c>
       <c r="K4" s="2">
+        <f t="shared" ref="K4:K47" si="1">(J4-M4)/L3</f>
         <v>1</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4">
+        <f t="shared" ref="L4:L47" si="2">L3+M4/K4</f>
+        <v>300000</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
         <v>1</v>
       </c>
-      <c r="M4" s="2">
-        <v>300000</v>
-      </c>
-      <c r="N4" s="2">
-        <v>300000</v>
-      </c>
-      <c r="O4" s="2">
-        <v>300000</v>
-      </c>
-      <c r="P4" s="2">
-        <v>300000</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="1">
+      <c r="O4" s="4">
+        <v>1</v>
+      </c>
+      <c r="P4" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R4" s="5">
+        <v>300000</v>
+      </c>
+      <c r="S4" s="4">
+        <v>300000</v>
+      </c>
+      <c r="T4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="3">
         <v>45661</v>
       </c>
       <c r="B5">
@@ -1272,34 +1335,45 @@
       <c r="I5">
         <v>3.9</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="1">
         <f t="shared" si="0"/>
         <v>300000</v>
       </c>
       <c r="K5" s="2">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
         <v>1</v>
       </c>
-      <c r="M5" s="2">
-        <v>300000</v>
-      </c>
-      <c r="N5" s="2">
-        <v>300000</v>
-      </c>
-      <c r="O5" s="2">
-        <v>300000</v>
-      </c>
-      <c r="P5" s="2">
-        <v>300000</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="1">
+      <c r="O5" s="4">
+        <v>1</v>
+      </c>
+      <c r="P5" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R5" s="5">
+        <v>300000</v>
+      </c>
+      <c r="S5" s="4">
+        <v>300000</v>
+      </c>
+      <c r="T5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="3">
         <v>45662</v>
       </c>
       <c r="B6">
@@ -1318,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H6">
         <v>380</v>
@@ -1326,34 +1400,45 @@
       <c r="I6">
         <v>3.9</v>
       </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>304800</v>
+      <c r="J6" s="1">
+        <f t="shared" si="0"/>
+        <v>299800</v>
       </c>
       <c r="K6" s="2">
+        <f t="shared" si="1"/>
+        <v>0.999333333333333</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="4">
         <v>0.999333</v>
       </c>
-      <c r="L6" s="2">
+      <c r="O6" s="4">
         <v>1</v>
       </c>
-      <c r="M6" s="2">
-        <v>300000</v>
-      </c>
-      <c r="N6" s="2">
-        <v>300000</v>
-      </c>
-      <c r="O6" s="2">
+      <c r="P6" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R6" s="5">
         <v>299800</v>
       </c>
-      <c r="P6" s="2">
-        <v>300000</v>
-      </c>
-      <c r="Q6" s="2">
+      <c r="S6" s="4">
+        <v>300000</v>
+      </c>
+      <c r="T6" s="4">
         <v>-0.0007</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="1">
+    <row r="7" spans="1:20">
+      <c r="A7" s="3">
         <v>45663</v>
       </c>
       <c r="B7">
@@ -1372,7 +1457,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H7">
         <v>380</v>
@@ -1380,34 +1465,45 @@
       <c r="I7">
         <v>3.9</v>
       </c>
-      <c r="J7">
-        <f t="shared" si="0"/>
-        <v>304800</v>
+      <c r="J7" s="1">
+        <f t="shared" si="0"/>
+        <v>299800</v>
       </c>
       <c r="K7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.999333333333333</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4">
         <v>0.999333</v>
       </c>
-      <c r="L7" s="2">
+      <c r="O7" s="4">
         <v>0.999333</v>
       </c>
-      <c r="M7" s="2">
-        <v>300000</v>
-      </c>
-      <c r="N7" s="2">
-        <v>300000</v>
-      </c>
-      <c r="O7" s="2">
+      <c r="P7" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R7" s="5">
         <v>299800</v>
       </c>
-      <c r="P7" s="2">
+      <c r="S7" s="4">
         <v>299800</v>
       </c>
-      <c r="Q7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" s="1">
+      <c r="T7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="3">
         <v>45664</v>
       </c>
       <c r="B8">
@@ -1426,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H8">
         <v>380</v>
@@ -1434,34 +1530,45 @@
       <c r="I8">
         <v>3.9</v>
       </c>
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>304800</v>
+      <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>299800</v>
       </c>
       <c r="K8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.999333333333333</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
         <v>0.999333</v>
       </c>
-      <c r="L8" s="2">
+      <c r="O8" s="4">
         <v>0.999333</v>
       </c>
-      <c r="M8" s="2">
-        <v>300000</v>
-      </c>
-      <c r="N8" s="2">
-        <v>300000</v>
-      </c>
-      <c r="O8" s="2">
+      <c r="P8" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R8" s="5">
         <v>299800</v>
       </c>
-      <c r="P8" s="2">
+      <c r="S8" s="4">
         <v>299800</v>
       </c>
-      <c r="Q8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="A9" s="1">
+      <c r="T8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="3">
         <v>45665</v>
       </c>
       <c r="B9">
@@ -1480,7 +1587,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H9">
         <v>380</v>
@@ -1488,34 +1595,45 @@
       <c r="I9">
         <v>3.9</v>
       </c>
-      <c r="J9">
-        <f t="shared" si="0"/>
-        <v>304800</v>
+      <c r="J9" s="1">
+        <f t="shared" si="0"/>
+        <v>299800</v>
       </c>
       <c r="K9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.999333333333333</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4">
         <v>0.999333</v>
       </c>
-      <c r="L9" s="2">
+      <c r="O9" s="4">
         <v>0.999333</v>
       </c>
-      <c r="M9" s="2">
-        <v>300000</v>
-      </c>
-      <c r="N9" s="2">
-        <v>300000</v>
-      </c>
-      <c r="O9" s="2">
+      <c r="P9" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R9" s="5">
         <v>299800</v>
       </c>
-      <c r="P9" s="2">
+      <c r="S9" s="4">
         <v>299800</v>
       </c>
-      <c r="Q9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="A10" s="1">
+      <c r="T9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="3">
         <v>45666</v>
       </c>
       <c r="B10">
@@ -1535,7 +1653,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H10">
         <v>380</v>
@@ -1543,34 +1661,45 @@
       <c r="I10">
         <v>3.9</v>
       </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>320800</v>
+      <c r="J10" s="1">
+        <f t="shared" si="0"/>
+        <v>299800</v>
       </c>
       <c r="K10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.999333333333333</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10" s="4">
         <v>0.999333</v>
       </c>
-      <c r="L10" s="2">
+      <c r="O10" s="4">
         <v>0.999333</v>
       </c>
-      <c r="M10" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N10" s="2">
-        <v>300000</v>
-      </c>
-      <c r="O10" s="2">
+      <c r="P10" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R10" s="5">
         <v>299800</v>
       </c>
-      <c r="P10" s="2">
+      <c r="S10" s="4">
         <v>299800</v>
       </c>
-      <c r="Q10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="1">
+      <c r="T10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="3">
         <v>45667</v>
       </c>
       <c r="B11">
@@ -1597,34 +1726,45 @@
       <c r="I11">
         <v>3.9</v>
       </c>
-      <c r="J11">
-        <f t="shared" si="0"/>
-        <v>320800</v>
+      <c r="J11" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K11" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L11" s="2">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O11" s="4">
         <v>0.999333</v>
       </c>
-      <c r="M11" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N11" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O11" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P11" s="2">
+      <c r="P11" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R11" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S11" s="4">
         <v>299800</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="T11" s="4">
         <v>0.0167</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
-      <c r="A12" s="1">
+    <row r="12" spans="1:20">
+      <c r="A12" s="3">
         <v>45668</v>
       </c>
       <c r="B12">
@@ -1652,34 +1792,45 @@
       <c r="I12">
         <v>3.9</v>
       </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J12" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K12" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L12" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M12" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N12" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O12" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P12" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="A13" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O12" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P12" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R12" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S12" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="3">
         <v>45669</v>
       </c>
       <c r="B13">
@@ -1706,34 +1857,45 @@
       <c r="I13">
         <v>3.9</v>
       </c>
-      <c r="J13">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J13" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K13" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L13" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M13" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N13" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O13" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P13" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="A14" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O13" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P13" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R13" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S13" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="3">
         <v>45670</v>
       </c>
       <c r="B14">
@@ -1760,34 +1922,45 @@
       <c r="I14">
         <v>3.9</v>
       </c>
-      <c r="J14">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J14" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K14" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L14" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M14" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N14" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O14" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P14" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="A15" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O14" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P14" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R14" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S14" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="3">
         <v>45671</v>
       </c>
       <c r="B15">
@@ -1814,34 +1987,45 @@
       <c r="I15">
         <v>3.9</v>
       </c>
-      <c r="J15">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J15" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K15" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L15" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M15" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N15" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O15" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P15" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q15" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="A16" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O15" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P15" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R15" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S15" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="3">
         <v>45672</v>
       </c>
       <c r="B16">
@@ -1868,34 +2052,45 @@
       <c r="I16">
         <v>3.9</v>
       </c>
-      <c r="J16">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J16" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K16" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L16" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M16" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N16" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O16" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P16" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q16" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
-      <c r="A17" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O16" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P16" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R16" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S16" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" s="3">
         <v>45673</v>
       </c>
       <c r="B17">
@@ -1922,34 +2117,45 @@
       <c r="I17">
         <v>3.9</v>
       </c>
-      <c r="J17">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J17" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K17" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L17" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M17" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N17" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O17" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P17" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q17" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="A18" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O17" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P17" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R17" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S17" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" s="3">
         <v>45674</v>
       </c>
       <c r="B18">
@@ -1976,34 +2182,45 @@
       <c r="I18">
         <v>3.9</v>
       </c>
-      <c r="J18">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J18" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K18" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L18" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M18" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N18" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O18" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P18" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q18" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="A19" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O18" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P18" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R18" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S18" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" s="3">
         <v>45675</v>
       </c>
       <c r="B19">
@@ -2030,34 +2247,45 @@
       <c r="I19">
         <v>3.9</v>
       </c>
-      <c r="J19">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J19" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K19" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L19" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M19" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N19" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O19" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P19" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q19" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
-      <c r="A20" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O19" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P19" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R19" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S19" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" s="3">
         <v>45676</v>
       </c>
       <c r="B20">
@@ -2084,34 +2312,45 @@
       <c r="I20">
         <v>3.9</v>
       </c>
-      <c r="J20">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J20" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K20" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L20" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M20" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N20" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O20" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P20" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q20" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17">
-      <c r="A21" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O20" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P20" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R20" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S20" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="3">
         <v>45677</v>
       </c>
       <c r="B21">
@@ -2138,34 +2377,45 @@
       <c r="I21">
         <v>3.9</v>
       </c>
-      <c r="J21">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J21" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K21" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L21" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M21" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N21" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O21" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P21" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q21" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17">
-      <c r="A22" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O21" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P21" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R21" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S21" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="3">
         <v>45678</v>
       </c>
       <c r="B22">
@@ -2192,34 +2442,45 @@
       <c r="I22">
         <v>3.9</v>
       </c>
-      <c r="J22">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J22" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K22" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L22" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M22" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N22" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O22" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P22" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q22" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17">
-      <c r="A23" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O22" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P22" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R22" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S22" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="3">
         <v>45679</v>
       </c>
       <c r="B23">
@@ -2246,34 +2507,45 @@
       <c r="I23">
         <v>3.9</v>
       </c>
-      <c r="J23">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J23" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K23" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L23" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M23" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N23" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O23" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P23" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q23" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17">
-      <c r="A24" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O23" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P23" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R23" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S23" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T23" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="3">
         <v>45680</v>
       </c>
       <c r="B24">
@@ -2300,34 +2572,45 @@
       <c r="I24">
         <v>3.9</v>
       </c>
-      <c r="J24">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J24" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K24" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L24" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M24" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N24" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O24" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P24" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q24" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17">
-      <c r="A25" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O24" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P24" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R24" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S24" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T24" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="3">
         <v>45681</v>
       </c>
       <c r="B25">
@@ -2354,34 +2637,45 @@
       <c r="I25">
         <v>3.9</v>
       </c>
-      <c r="J25">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J25" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K25" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L25" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M25" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N25" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O25" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P25" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q25" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17">
-      <c r="A26" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O25" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P25" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R25" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S25" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="3">
         <v>45682</v>
       </c>
       <c r="B26">
@@ -2408,34 +2702,45 @@
       <c r="I26">
         <v>3.9</v>
       </c>
-      <c r="J26">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J26" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K26" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L26" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M26" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N26" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O26" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P26" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q26" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17">
-      <c r="A27" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O26" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P26" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R26" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S26" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="3">
         <v>45683</v>
       </c>
       <c r="B27">
@@ -2462,34 +2767,45 @@
       <c r="I27">
         <v>3.9</v>
       </c>
-      <c r="J27">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J27" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K27" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L27" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M27" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N27" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O27" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P27" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q27" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17">
-      <c r="A28" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O27" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P27" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R27" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S27" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T27" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="3">
         <v>45684</v>
       </c>
       <c r="B28">
@@ -2516,34 +2832,45 @@
       <c r="I28">
         <v>3.9</v>
       </c>
-      <c r="J28">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J28" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K28" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L28" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M28" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N28" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O28" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P28" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q28" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17">
-      <c r="A29" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O28" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P28" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R28" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S28" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T28" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="3">
         <v>45685</v>
       </c>
       <c r="B29">
@@ -2570,34 +2897,45 @@
       <c r="I29">
         <v>3.9</v>
       </c>
-      <c r="J29">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J29" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K29" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L29" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M29" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N29" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O29" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P29" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q29" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
-      <c r="A30" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O29" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P29" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q29" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R29" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S29" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="3">
         <v>45686</v>
       </c>
       <c r="B30">
@@ -2624,34 +2962,45 @@
       <c r="I30">
         <v>3.9</v>
       </c>
-      <c r="J30">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J30" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K30" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L30" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M30" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N30" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O30" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P30" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q30" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="A31" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O30" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P30" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R30" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S30" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T30" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31" s="3">
         <v>45687</v>
       </c>
       <c r="B31">
@@ -2678,34 +3027,45 @@
       <c r="I31">
         <v>3.9</v>
       </c>
-      <c r="J31">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J31" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K31" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L31" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M31" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N31" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O31" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P31" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q31" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17">
-      <c r="A32" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O31" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P31" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q31" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R31" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S31" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T31" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32" s="3">
         <v>45688</v>
       </c>
       <c r="B32">
@@ -2732,38 +3092,49 @@
       <c r="I32">
         <v>3.9</v>
       </c>
-      <c r="J32">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J32" s="1">
+        <f t="shared" si="0"/>
+        <v>304800</v>
       </c>
       <c r="K32" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L32" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M32" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N32" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O32" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P32" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q32" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17">
-      <c r="A33" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="2"/>
+        <v>300000</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O32" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P32" s="4">
+        <v>300000</v>
+      </c>
+      <c r="Q32" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R32" s="5">
+        <v>304800</v>
+      </c>
+      <c r="S32" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T32" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20">
+      <c r="A33" s="3">
         <v>45689</v>
       </c>
       <c r="B33">
-        <v>80800</v>
+        <v>180800</v>
       </c>
       <c r="C33">
         <v>10000</v>
@@ -2786,38 +3157,49 @@
       <c r="I33">
         <v>3.9</v>
       </c>
-      <c r="J33">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J33" s="1">
+        <f t="shared" si="0"/>
+        <v>404800</v>
       </c>
       <c r="K33" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L33" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M33" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N33" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O33" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P33" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q33" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17">
-      <c r="A34" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="2"/>
+        <v>398425.196850394</v>
+      </c>
+      <c r="M33">
+        <v>100000</v>
+      </c>
+      <c r="N33" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O33" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P33" s="4">
+        <v>398425.2</v>
+      </c>
+      <c r="Q33" s="4">
+        <v>300000</v>
+      </c>
+      <c r="R33" s="5">
+        <v>404800</v>
+      </c>
+      <c r="S33" s="4">
+        <v>304800</v>
+      </c>
+      <c r="T33" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20">
+      <c r="A34" s="3">
         <v>45690</v>
       </c>
       <c r="B34">
-        <v>80800</v>
+        <v>180800</v>
       </c>
       <c r="C34">
         <v>10000</v>
@@ -2840,38 +3222,49 @@
       <c r="I34">
         <v>3.9</v>
       </c>
-      <c r="J34">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J34" s="1">
+        <f t="shared" si="0"/>
+        <v>404800</v>
       </c>
       <c r="K34" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L34" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M34" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N34" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O34" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P34" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q34" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17">
-      <c r="A35" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="2"/>
+        <v>398425.196850394</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O34" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P34" s="4">
+        <v>398425.2</v>
+      </c>
+      <c r="Q34" s="4">
+        <v>398425.2</v>
+      </c>
+      <c r="R34" s="5">
+        <v>404800</v>
+      </c>
+      <c r="S34" s="4">
+        <v>404800</v>
+      </c>
+      <c r="T34" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20">
+      <c r="A35" s="3">
         <v>45691</v>
       </c>
       <c r="B35">
-        <v>80800</v>
+        <v>180800</v>
       </c>
       <c r="C35">
         <v>10000</v>
@@ -2894,38 +3287,49 @@
       <c r="I35">
         <v>3.9</v>
       </c>
-      <c r="J35">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J35" s="1">
+        <f t="shared" si="0"/>
+        <v>404800</v>
       </c>
       <c r="K35" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L35" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M35" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N35" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O35" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P35" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q35" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17">
-      <c r="A36" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="2"/>
+        <v>398425.196850394</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O35" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P35" s="4">
+        <v>398425.2</v>
+      </c>
+      <c r="Q35" s="4">
+        <v>398425.2</v>
+      </c>
+      <c r="R35" s="5">
+        <v>404800</v>
+      </c>
+      <c r="S35" s="4">
+        <v>404800</v>
+      </c>
+      <c r="T35" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20">
+      <c r="A36" s="3">
         <v>45692</v>
       </c>
       <c r="B36">
-        <v>80800</v>
+        <v>180800</v>
       </c>
       <c r="C36">
         <v>10000</v>
@@ -2948,38 +3352,49 @@
       <c r="I36">
         <v>3.9</v>
       </c>
-      <c r="J36">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J36" s="1">
+        <f t="shared" si="0"/>
+        <v>404800</v>
       </c>
       <c r="K36" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L36" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M36" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N36" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O36" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P36" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q36" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17">
-      <c r="A37" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="2"/>
+        <v>398425.196850394</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O36" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P36" s="4">
+        <v>398425.2</v>
+      </c>
+      <c r="Q36" s="4">
+        <v>398425.2</v>
+      </c>
+      <c r="R36" s="5">
+        <v>404800</v>
+      </c>
+      <c r="S36" s="4">
+        <v>404800</v>
+      </c>
+      <c r="T36" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20">
+      <c r="A37" s="3">
         <v>45693</v>
       </c>
       <c r="B37">
-        <v>80800</v>
+        <v>180800</v>
       </c>
       <c r="C37">
         <v>10000</v>
@@ -3002,38 +3417,49 @@
       <c r="I37">
         <v>3.9</v>
       </c>
-      <c r="J37">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J37" s="1">
+        <f t="shared" si="0"/>
+        <v>404800</v>
       </c>
       <c r="K37" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L37" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M37" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N37" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O37" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P37" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q37" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17">
-      <c r="A38" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="2"/>
+        <v>398425.196850394</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O37" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P37" s="4">
+        <v>398425.2</v>
+      </c>
+      <c r="Q37" s="4">
+        <v>398425.2</v>
+      </c>
+      <c r="R37" s="5">
+        <v>404800</v>
+      </c>
+      <c r="S37" s="4">
+        <v>404800</v>
+      </c>
+      <c r="T37" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20">
+      <c r="A38" s="3">
         <v>45694</v>
       </c>
       <c r="B38">
-        <v>80800</v>
+        <v>180800</v>
       </c>
       <c r="C38">
         <v>10000</v>
@@ -3056,38 +3482,50 @@
       <c r="I38">
         <v>3.9</v>
       </c>
-      <c r="J38">
-        <f t="shared" si="0"/>
-        <v>305600</v>
+      <c r="J38" s="1">
+        <f t="shared" si="0"/>
+        <v>404800</v>
       </c>
       <c r="K38" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="L38" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M38" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N38" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O38" s="2">
-        <v>304800</v>
-      </c>
-      <c r="P38" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q38" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17">
-      <c r="A39" s="1">
+        <f t="shared" si="1"/>
+        <v>1.016</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="2"/>
+        <v>398425.196850394</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="O38" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P38" s="4">
+        <v>398425.2</v>
+      </c>
+      <c r="Q38" s="4">
+        <v>398425.2</v>
+      </c>
+      <c r="R38" s="5">
+        <v>404800</v>
+      </c>
+      <c r="S38" s="4">
+        <v>404800</v>
+      </c>
+      <c r="T38" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20">
+      <c r="A39" s="3">
         <v>45695</v>
       </c>
       <c r="B39">
-        <v>80900</v>
+        <f>B38+100</f>
+        <v>180900</v>
       </c>
       <c r="C39">
         <v>10000</v>
@@ -3110,41 +3548,52 @@
       <c r="I39">
         <v>3.9</v>
       </c>
-      <c r="J39">
-        <f t="shared" si="0"/>
-        <v>310700</v>
+      <c r="J39" s="1">
+        <f t="shared" si="0"/>
+        <v>409900</v>
       </c>
       <c r="K39" s="2">
-        <v>0.980663</v>
-      </c>
-      <c r="L39" s="2">
-        <v>0.964524</v>
-      </c>
-      <c r="M39" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N39" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O39" s="2">
-        <v>309900</v>
-      </c>
-      <c r="P39" s="2">
-        <v>304800</v>
-      </c>
-      <c r="Q39" s="2">
-        <v>0.0167</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17">
-      <c r="A40" s="1">
+        <f t="shared" si="1"/>
+        <v>1.02880039525692</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="2"/>
+        <v>398425.196850394</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39" s="4">
+        <v>1.0288</v>
+      </c>
+      <c r="O39" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="P39" s="4">
+        <v>398425.2</v>
+      </c>
+      <c r="Q39" s="4">
+        <v>398425.2</v>
+      </c>
+      <c r="R39" s="5">
+        <v>409900</v>
+      </c>
+      <c r="S39" s="4">
+        <v>404800</v>
+      </c>
+      <c r="T39" s="4">
+        <v>0.0126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20">
+      <c r="A40" s="3">
         <v>45696</v>
       </c>
       <c r="B40">
-        <v>80900</v>
+        <v>180900</v>
       </c>
       <c r="C40">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="D40">
         <v>1000</v>
@@ -3164,41 +3613,52 @@
       <c r="I40">
         <v>3.9</v>
       </c>
-      <c r="J40">
-        <f t="shared" si="0"/>
-        <v>310700</v>
+      <c r="J40" s="1">
+        <f t="shared" si="0"/>
+        <v>400700</v>
       </c>
       <c r="K40" s="2">
-        <v>0.980663</v>
-      </c>
-      <c r="L40" s="2">
-        <v>0.980663</v>
-      </c>
-      <c r="M40" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N40" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O40" s="2">
-        <v>309900</v>
-      </c>
-      <c r="P40" s="2">
-        <v>309900</v>
-      </c>
-      <c r="Q40" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17">
-      <c r="A41" s="1">
+        <f t="shared" si="1"/>
+        <v>1.02880039525692</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="2"/>
+        <v>389482.743054288</v>
+      </c>
+      <c r="M40">
+        <v>-9200</v>
+      </c>
+      <c r="N40" s="4">
+        <v>1.0288</v>
+      </c>
+      <c r="O40" s="4">
+        <v>1.0288</v>
+      </c>
+      <c r="P40" s="4">
+        <v>389482.74</v>
+      </c>
+      <c r="Q40" s="4">
+        <v>398425.2</v>
+      </c>
+      <c r="R40" s="5">
+        <v>400700</v>
+      </c>
+      <c r="S40" s="4">
+        <v>409900</v>
+      </c>
+      <c r="T40" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20">
+      <c r="A41" s="3">
         <v>45697</v>
       </c>
       <c r="B41">
-        <v>80900</v>
+        <v>180900</v>
       </c>
       <c r="C41">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="D41">
         <v>1000</v>
@@ -3218,42 +3678,53 @@
       <c r="I41">
         <v>3.9</v>
       </c>
-      <c r="J41">
-        <f t="shared" si="0"/>
-        <v>310700</v>
+      <c r="J41" s="1">
+        <f t="shared" si="0"/>
+        <v>400700</v>
       </c>
       <c r="K41" s="2">
-        <v>0.980663</v>
-      </c>
-      <c r="L41" s="2">
-        <v>0.980663</v>
-      </c>
-      <c r="M41" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N41" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O41" s="2">
-        <v>309900</v>
-      </c>
-      <c r="P41" s="2">
-        <v>309900</v>
-      </c>
-      <c r="Q41" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17">
-      <c r="A42" s="1">
+        <f t="shared" si="1"/>
+        <v>1.02880039525692</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="2"/>
+        <v>389482.743054288</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41" s="4">
+        <v>1.0288</v>
+      </c>
+      <c r="O41" s="4">
+        <v>1.0288</v>
+      </c>
+      <c r="P41" s="4">
+        <v>389482.74</v>
+      </c>
+      <c r="Q41" s="4">
+        <v>389482.74</v>
+      </c>
+      <c r="R41" s="5">
+        <v>400700</v>
+      </c>
+      <c r="S41" s="4">
+        <v>400700</v>
+      </c>
+      <c r="T41" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20">
+      <c r="A42" s="3">
         <v>45698</v>
       </c>
       <c r="B42">
         <f>B41+48000</f>
-        <v>128900</v>
+        <v>228900</v>
       </c>
       <c r="C42">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -3273,42 +3744,53 @@
       <c r="I42">
         <v>3.9</v>
       </c>
-      <c r="J42">
-        <f t="shared" si="0"/>
-        <v>313700</v>
+      <c r="J42" s="1">
+        <f t="shared" si="0"/>
+        <v>403700</v>
       </c>
       <c r="K42" s="2">
-        <v>0.990156</v>
-      </c>
-      <c r="L42" s="2">
-        <v>0.980663</v>
-      </c>
-      <c r="M42" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N42" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O42" s="2">
-        <v>312900</v>
-      </c>
-      <c r="P42" s="2">
-        <v>309900</v>
-      </c>
-      <c r="Q42" s="2">
-        <v>0.0097</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17">
-      <c r="A43" s="1">
+        <f t="shared" si="1"/>
+        <v>1.03650291880513</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="2"/>
+        <v>389482.743054288</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42" s="4">
+        <v>1.036503</v>
+      </c>
+      <c r="O42" s="4">
+        <v>1.0288</v>
+      </c>
+      <c r="P42" s="4">
+        <v>389482.74</v>
+      </c>
+      <c r="Q42" s="4">
+        <v>389482.74</v>
+      </c>
+      <c r="R42" s="5">
+        <v>403700</v>
+      </c>
+      <c r="S42" s="4">
+        <v>400700</v>
+      </c>
+      <c r="T42" s="4">
+        <v>0.0075</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20">
+      <c r="A43" s="3">
         <v>45699</v>
       </c>
       <c r="B43">
-        <v>128900</v>
+        <v>228900</v>
       </c>
       <c r="C43">
         <f>C42+40000</f>
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -3328,42 +3810,53 @@
       <c r="I43">
         <v>3.9</v>
       </c>
-      <c r="J43">
-        <f t="shared" si="0"/>
-        <v>344500</v>
+      <c r="J43" s="1">
+        <f t="shared" si="0"/>
+        <v>431300</v>
       </c>
       <c r="K43" s="2">
-        <v>1.077495</v>
-      </c>
-      <c r="L43" s="2">
-        <v>0.990156</v>
-      </c>
-      <c r="M43" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N43" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O43" s="2">
-        <v>340500</v>
-      </c>
-      <c r="P43" s="2">
-        <v>312900</v>
-      </c>
-      <c r="Q43" s="2">
-        <v>0.0882</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17">
-      <c r="A44" s="1">
+        <f t="shared" si="1"/>
+        <v>1.10736613544874</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="2"/>
+        <v>389482.743054288</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43" s="4">
+        <v>1.107366</v>
+      </c>
+      <c r="O43" s="4">
+        <v>1.036503</v>
+      </c>
+      <c r="P43" s="4">
+        <v>389482.74</v>
+      </c>
+      <c r="Q43" s="4">
+        <v>389482.74</v>
+      </c>
+      <c r="R43" s="5">
+        <v>431300</v>
+      </c>
+      <c r="S43" s="4">
+        <v>403700</v>
+      </c>
+      <c r="T43" s="4">
+        <v>0.0684</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20">
+      <c r="A44" s="3">
         <v>45700</v>
       </c>
       <c r="B44">
         <f>B43-38000</f>
-        <v>90900</v>
+        <v>190900</v>
       </c>
       <c r="C44">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -3383,41 +3876,52 @@
       <c r="I44">
         <v>3.9</v>
       </c>
-      <c r="J44">
-        <f t="shared" si="0"/>
-        <v>345500</v>
+      <c r="J44" s="1">
+        <f t="shared" si="0"/>
+        <v>432300</v>
       </c>
       <c r="K44" s="2">
-        <v>1.08066</v>
-      </c>
-      <c r="L44" s="2">
-        <v>1.077495</v>
-      </c>
-      <c r="M44" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N44" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O44" s="2">
-        <v>341500</v>
-      </c>
-      <c r="P44" s="2">
-        <v>340500</v>
-      </c>
-      <c r="Q44" s="2">
-        <v>0.0029</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17">
-      <c r="A45" s="1">
+        <f t="shared" si="1"/>
+        <v>1.10993364329814</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="2"/>
+        <v>389482.743054288</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44" s="4">
+        <v>1.109934</v>
+      </c>
+      <c r="O44" s="4">
+        <v>1.107366</v>
+      </c>
+      <c r="P44" s="4">
+        <v>389482.74</v>
+      </c>
+      <c r="Q44" s="4">
+        <v>389482.74</v>
+      </c>
+      <c r="R44" s="5">
+        <v>432300</v>
+      </c>
+      <c r="S44" s="4">
+        <v>431300</v>
+      </c>
+      <c r="T44" s="4">
+        <v>0.0023</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20">
+      <c r="A45" s="3">
         <v>45701</v>
       </c>
       <c r="B45">
-        <v>90900</v>
+        <v>190900</v>
       </c>
       <c r="C45">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -3437,41 +3941,52 @@
       <c r="I45">
         <v>3.9</v>
       </c>
-      <c r="J45">
-        <f t="shared" si="0"/>
-        <v>345500</v>
+      <c r="J45" s="1">
+        <f t="shared" si="0"/>
+        <v>432300</v>
       </c>
       <c r="K45" s="2">
-        <v>1.08066</v>
-      </c>
-      <c r="L45" s="2">
-        <v>1.08066</v>
-      </c>
-      <c r="M45" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N45" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O45" s="2">
-        <v>341500</v>
-      </c>
-      <c r="P45" s="2">
-        <v>341500</v>
-      </c>
-      <c r="Q45" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17">
-      <c r="A46" s="1">
+        <f t="shared" si="1"/>
+        <v>1.10993364329814</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="2"/>
+        <v>389482.743054288</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45" s="4">
+        <v>1.109934</v>
+      </c>
+      <c r="O45" s="4">
+        <v>1.109934</v>
+      </c>
+      <c r="P45" s="4">
+        <v>389482.74</v>
+      </c>
+      <c r="Q45" s="4">
+        <v>389482.74</v>
+      </c>
+      <c r="R45" s="5">
+        <v>432300</v>
+      </c>
+      <c r="S45" s="4">
+        <v>432300</v>
+      </c>
+      <c r="T45" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20">
+      <c r="A46" s="3">
         <v>45702</v>
       </c>
       <c r="B46">
-        <v>90900</v>
+        <v>190900</v>
       </c>
       <c r="C46">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -3491,41 +4006,52 @@
       <c r="I46">
         <v>3.9</v>
       </c>
-      <c r="J46">
-        <f t="shared" si="0"/>
-        <v>345500</v>
+      <c r="J46" s="1">
+        <f t="shared" si="0"/>
+        <v>432300</v>
       </c>
       <c r="K46" s="2">
-        <v>1.08066</v>
-      </c>
-      <c r="L46" s="2">
-        <v>1.08066</v>
-      </c>
-      <c r="M46" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N46" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O46" s="2">
-        <v>341500</v>
-      </c>
-      <c r="P46" s="2">
-        <v>341500</v>
-      </c>
-      <c r="Q46" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17">
-      <c r="A47" s="1">
+        <f t="shared" si="1"/>
+        <v>1.10993364329814</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="2"/>
+        <v>389482.743054288</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46" s="4">
+        <v>1.109934</v>
+      </c>
+      <c r="O46" s="4">
+        <v>1.109934</v>
+      </c>
+      <c r="P46" s="4">
+        <v>389482.74</v>
+      </c>
+      <c r="Q46" s="4">
+        <v>389482.74</v>
+      </c>
+      <c r="R46" s="5">
+        <v>432300</v>
+      </c>
+      <c r="S46" s="4">
+        <v>432300</v>
+      </c>
+      <c r="T46" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20">
+      <c r="A47" s="3">
         <v>45703</v>
       </c>
       <c r="B47">
-        <v>90900</v>
+        <v>190900</v>
       </c>
       <c r="C47">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -3545,29 +4071,40 @@
       <c r="I47">
         <v>3.9</v>
       </c>
-      <c r="J47">
-        <f t="shared" si="0"/>
-        <v>345500</v>
+      <c r="J47" s="1">
+        <f t="shared" si="0"/>
+        <v>432300</v>
       </c>
       <c r="K47" s="2">
-        <v>1.08066</v>
-      </c>
-      <c r="L47" s="2">
-        <v>1.08066</v>
-      </c>
-      <c r="M47" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="N47" s="2">
-        <v>316010.67</v>
-      </c>
-      <c r="O47" s="2">
-        <v>341500</v>
-      </c>
-      <c r="P47" s="2">
-        <v>341500</v>
-      </c>
-      <c r="Q47" s="2">
+        <f t="shared" si="1"/>
+        <v>1.10993364329814</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="2"/>
+        <v>389482.743054288</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47" s="4">
+        <v>1.109934</v>
+      </c>
+      <c r="O47" s="4">
+        <v>1.109934</v>
+      </c>
+      <c r="P47" s="4">
+        <v>389482.74</v>
+      </c>
+      <c r="Q47" s="4">
+        <v>389482.74</v>
+      </c>
+      <c r="R47" s="5">
+        <v>432300</v>
+      </c>
+      <c r="S47" s="4">
+        <v>432300</v>
+      </c>
+      <c r="T47" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>